<commit_message>
chore: updated ablation details
</commit_message>
<xml_diff>
--- a/report/model_comparison.xlsx
+++ b/report/model_comparison.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gopikrishnan.Srinivasan@ey.com/Library/Mobile Documents/com~apple~CloudDocs/Documents/UIUC/Courses/CS598-Deep-Learning/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/gopikrishnan_srinivasan_ey_com/Documents/Gopi/UIUC/DLH/ConvolutionMedicalNer/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8BF79FE-5C49-0F41-BF5B-BE95BF321497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51440" yWindow="1460" windowWidth="28040" windowHeight="17440" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
+    <workbookView xWindow="46520" yWindow="960" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
   </bookViews>
   <sheets>
     <sheet name="proposed" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Baseline sorting'!$P$1:$S$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Timeseries!$A$1:$E$9</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="71">
   <si>
     <t>Task</t>
   </si>
@@ -236,13 +236,34 @@
   </si>
   <si>
     <t>Glove</t>
+  </si>
+  <si>
+    <t>Proposed AUPRC</t>
+  </si>
+  <si>
+    <t>% vs multimodal</t>
+  </si>
+  <si>
+    <t>% vs timeseries</t>
+  </si>
+  <si>
+    <t>In-hospital</t>
+  </si>
+  <si>
+    <t>los &gt; 3</t>
+  </si>
+  <si>
+    <t>los &gt; 7</t>
+  </si>
+  <si>
+    <t>icu mort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,8 +285,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,8 +306,13 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -351,12 +385,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -384,6 +434,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -393,11 +446,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -713,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6912B902-6D37-5449-8B39-71DCD8060D35}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -743,7 +798,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -752,19 +807,19 @@
       <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="11">
         <v>0.87530068728522303</v>
       </c>
-      <c r="E2" s="14">
+      <c r="E2" s="11">
         <v>0.57982780097661202</v>
       </c>
-      <c r="F2" s="14">
+      <c r="F2" s="11">
         <v>0.47246376811594198</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="12"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="15"/>
+      <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -776,13 +831,13 @@
       <c r="E3" s="5">
         <v>0.57975787210374596</v>
       </c>
-      <c r="F3" s="16">
+      <c r="F3" s="13">
         <v>0.49450549450549403</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="12"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="15"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
@@ -797,15 +852,15 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="16"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="16">
+      <c r="D5" s="13">
         <v>0.87878943078685301</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>0.58014632667510002</v>
       </c>
       <c r="F5" s="5">
@@ -813,7 +868,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -833,8 +888,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="10" t="s">
+      <c r="A7" s="15"/>
+      <c r="B7" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -851,8 +906,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="12"/>
-      <c r="B8" s="10"/>
+      <c r="A8" s="15"/>
+      <c r="B8" s="17"/>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
@@ -867,8 +922,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="16"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
@@ -878,12 +933,12 @@
       <c r="E9" s="5">
         <v>0.51882856484952999</v>
       </c>
-      <c r="F9" s="16">
+      <c r="F9" s="13">
         <v>0.45726495726495697</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -903,17 +958,17 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="12"/>
-      <c r="B11" s="10" t="s">
+      <c r="A11" s="15"/>
+      <c r="B11" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16">
+      <c r="D11" s="13">
         <v>0.702856581769842</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>0.64664572030138301</v>
       </c>
       <c r="F11" s="5">
@@ -921,8 +976,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
-      <c r="B12" s="10"/>
+      <c r="A12" s="15"/>
+      <c r="B12" s="17"/>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
@@ -937,8 +992,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="10"/>
+      <c r="A13" s="16"/>
+      <c r="B13" s="17"/>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
@@ -953,7 +1008,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -973,14 +1028,14 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="15"/>
+      <c r="B15" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D15" s="13">
         <v>0.73612815518677799</v>
       </c>
       <c r="E15" s="5">
@@ -991,8 +1046,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
-      <c r="B16" s="12"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1007,18 +1062,18 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="16"/>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="5">
         <v>0.72857653509265696</v>
       </c>
-      <c r="E17" s="16">
+      <c r="E17" s="13">
         <v>0.226835014050909</v>
       </c>
-      <c r="F17" s="16">
+      <c r="F17" s="13">
         <v>3.2786885245901599E-2</v>
       </c>
     </row>
@@ -1457,7 +1512,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1474,7 +1529,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
+      <c r="A3" s="17"/>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1489,7 +1544,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
+      <c r="A4" s="17"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1504,7 +1559,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1519,7 +1574,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1536,7 +1591,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1606,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
+      <c r="A8" s="17"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1566,7 +1621,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
+      <c r="A9" s="17"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1581,7 +1636,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1598,7 +1653,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1613,7 +1668,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="10"/>
+      <c r="A12" s="17"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1628,7 +1683,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
+      <c r="A13" s="17"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1643,7 +1698,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1660,7 +1715,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
+      <c r="A15" s="17"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1675,7 +1730,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1690,7 +1745,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="10"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1719,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382CD632-0A6C-274D-974D-E990EBE38F8D}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1749,20 +1804,28 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="17" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
+      <c r="C2" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="11">
+        <v>0.87530068728522303</v>
+      </c>
+      <c r="E2" s="11">
+        <v>0.57982780097661202</v>
+      </c>
+      <c r="F2" s="11">
+        <v>0.47246376811594198</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="10"/>
-      <c r="B3" s="10" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1774,13 +1837,13 @@
       <c r="E3" s="5">
         <v>0.57975787210374596</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="13">
         <v>0.49450549450549403</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1795,8 +1858,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1811,17 +1874,17 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="10"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="13">
         <v>0.87769076915976596</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="13">
         <v>0.58175855132687204</v>
       </c>
       <c r="F6" s="5">
@@ -1829,20 +1892,28 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="17" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="13">
+        <v>0.88780373612996799</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.52652391224719597</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0.45614035087719301</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="10"/>
-      <c r="B8" s="10" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1859,8 +1930,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1875,8 +1946,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1891,7 +1962,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="10"/>
+      <c r="A11" s="17"/>
       <c r="B11" s="4" t="s">
         <v>62</v>
       </c>
@@ -1904,25 +1975,33 @@
       <c r="E11" s="5">
         <v>0.52588994937270295</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="13">
         <v>0.46220302375809902</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="17" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.70258855468227299</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.64359314820987201</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.57725947521865895</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1939,8 +2018,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
@@ -1955,8 +2034,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
       <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1971,44 +2050,52 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="10"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="4" t="s">
         <v>62</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="13">
         <v>0.71348302180900203</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="13">
         <v>0.65545219329892701</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="13">
         <v>0.56099843993759702</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="17" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
+      <c r="C17" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.72721848190763505</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.220187328008842</v>
+      </c>
+      <c r="F17" s="5">
+        <v>1.6483516483516401E-2</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="10"/>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="17"/>
+      <c r="B18" s="17" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="13">
         <v>0.73612815518677799</v>
       </c>
       <c r="E18" s="5">
@@ -2019,8 +2106,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="10"/>
-      <c r="B19" s="10"/>
+      <c r="A19" s="17"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="4" t="s">
         <v>10</v>
       </c>
@@ -2035,23 +2122,23 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
+      <c r="A20" s="17"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="5">
         <v>0.72857653509265696</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="13">
         <v>0.226835014050909</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="13">
         <v>3.2786885245901599E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="10"/>
+      <c r="A21" s="17"/>
       <c r="B21" s="4" t="s">
         <v>62</v>
       </c>
@@ -2085,10 +2172,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359A555D-11EF-2C4B-8DAD-F0A6302620A2}">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2151,13 +2238,13 @@
       <c r="A2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="11">
         <v>0.87530068728522303</v>
       </c>
-      <c r="C2" s="14">
+      <c r="C2" s="18">
         <v>0.57982780097661202</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="11">
         <v>0.47246376811594198</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -2166,7 +2253,7 @@
       <c r="G2" s="5">
         <v>0.88780373612996799</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="18">
         <v>0.52652391224719597</v>
       </c>
       <c r="I2" s="5">
@@ -2178,7 +2265,7 @@
       <c r="L2" s="5">
         <v>0.70258855468227299</v>
       </c>
-      <c r="M2" s="5">
+      <c r="M2" s="18">
         <v>0.64359314820987201</v>
       </c>
       <c r="N2" s="5">
@@ -2190,7 +2277,7 @@
       <c r="Q2" s="5">
         <v>0.72721848190763505</v>
       </c>
-      <c r="R2" s="5">
+      <c r="R2" s="18">
         <v>0.220187328008842</v>
       </c>
       <c r="S2" s="5">
@@ -2251,13 +2338,13 @@
       <c r="A4" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="12">
         <v>0.873989448</v>
       </c>
-      <c r="C4" s="15">
+      <c r="C4" s="12">
         <v>0.55767708199999999</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="12">
         <v>0.42813455700000003</v>
       </c>
       <c r="F4" s="8" t="s">
@@ -2345,6 +2432,79 @@
       </c>
       <c r="S5" s="5">
         <v>1.6348773841961799E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="13">
+        <v>0.58014632667510002</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0.51882856484952999</v>
+      </c>
+      <c r="D9" s="13">
+        <v>0.64664572030138301</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.226835014050909</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10">
+        <f>((B9-C2)/C2)*100</f>
+        <v>5.4934533658356217E-2</v>
+      </c>
+      <c r="C10">
+        <f>((C9-H2)/H2)*100</f>
+        <v>-1.4615380647808283</v>
+      </c>
+      <c r="D10">
+        <f>((D9-M2)/M2)*100</f>
+        <v>0.47430152107765611</v>
+      </c>
+      <c r="E10">
+        <f>((E9-R2)/R2)*100</f>
+        <v>3.0191047333114707</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>66</v>
+      </c>
+      <c r="B11">
+        <f>((B9-C4)/C4)*100</f>
+        <v>4.0290780095388659</v>
+      </c>
+      <c r="C11">
+        <f>((C9-H4)/H4)*100</f>
+        <v>7.3519489186830684</v>
+      </c>
+      <c r="D11">
+        <f>((D9-M5)/M5)*100</f>
+        <v>3.0798975113802682</v>
+      </c>
+      <c r="E11">
+        <f>((E9-R3)/R3)*100</f>
+        <v>10.382577597020793</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: new sheet for comparison
</commit_message>
<xml_diff>
--- a/report/model_comparison.xlsx
+++ b/report/model_comparison.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/gopikrishnan_srinivasan_ey_com/Documents/Gopi/UIUC/DLH/ConvolutionMedicalNer/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="136" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F2C8F355-CCFC-0A40-8AC9-F07C37246D67}"/>
   <bookViews>
-    <workbookView xWindow="46520" yWindow="960" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
+    <workbookView xWindow="30720" yWindow="-2940" windowWidth="51200" windowHeight="28800" activeTab="4" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
   </bookViews>
   <sheets>
     <sheet name="proposed" sheetId="1" r:id="rId1"/>
     <sheet name="model_results" sheetId="3" r:id="rId2"/>
     <sheet name="Timeseries" sheetId="2" r:id="rId3"/>
-    <sheet name="Baseline" sheetId="4" r:id="rId4"/>
+    <sheet name="Baseline models" sheetId="4" r:id="rId4"/>
     <sheet name="Ablation" sheetId="5" r:id="rId5"/>
     <sheet name="Baseline sorting" sheetId="6" r:id="rId6"/>
+    <sheet name="Comparison" sheetId="7" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Baseline sorting'!$P$1:$S$5</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="85">
   <si>
     <t>Task</t>
   </si>
@@ -238,9 +239,6 @@
     <t>Glove</t>
   </si>
   <si>
-    <t>Proposed AUPRC</t>
-  </si>
-  <si>
     <t>% vs multimodal</t>
   </si>
   <si>
@@ -257,13 +255,58 @@
   </si>
   <si>
     <t>icu mort</t>
+  </si>
+  <si>
+    <t>Glove (Ablation)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposed </t>
+  </si>
+  <si>
+    <t>Multimodal</t>
+  </si>
+  <si>
+    <t>TimeSeries</t>
+  </si>
+  <si>
+    <t>Ablation - Glove</t>
+  </si>
+  <si>
+    <t>proposed vs multimodal</t>
+  </si>
+  <si>
+    <t>proposed vs timeseries</t>
+  </si>
+  <si>
+    <t>glove vs multimodal</t>
+  </si>
+  <si>
+    <t>glove vs timeseries</t>
+  </si>
+  <si>
+    <t>Comparision %</t>
+  </si>
+  <si>
+    <t>golve vs proposed</t>
+  </si>
+  <si>
+    <t>In-Hospital</t>
+  </si>
+  <si>
+    <t>ICU mort</t>
+  </si>
+  <si>
+    <t>LOS &gt; 3</t>
+  </si>
+  <si>
+    <t>LOS &gt; 7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -289,6 +332,14 @@
       <b/>
       <sz val="12"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,7 +457,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -437,6 +488,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -449,7 +501,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -768,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6912B902-6D37-5449-8B39-71DCD8060D35}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="C2" sqref="C2:F2"/>
     </sheetView>
   </sheetViews>
@@ -798,7 +861,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="15" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -818,8 +881,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -836,8 +899,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="16"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
@@ -852,8 +915,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
@@ -868,7 +931,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="15" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
@@ -888,8 +951,8 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="17" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -906,8 +969,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="17"/>
+      <c r="A8" s="16"/>
+      <c r="B8" s="18"/>
       <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
@@ -922,8 +985,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="3" t="s">
         <v>11</v>
       </c>
@@ -938,7 +1001,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
@@ -958,8 +1021,8 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="17" t="s">
+      <c r="A11" s="16"/>
+      <c r="B11" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -976,8 +1039,8 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="17"/>
+      <c r="A12" s="16"/>
+      <c r="B12" s="18"/>
       <c r="C12" s="3" t="s">
         <v>10</v>
       </c>
@@ -992,8 +1055,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="17"/>
+      <c r="A13" s="17"/>
+      <c r="B13" s="18"/>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1008,7 +1071,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="14" t="s">
+      <c r="A14" s="15" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="3" t="s">
@@ -1028,8 +1091,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="14" t="s">
+      <c r="A15" s="16"/>
+      <c r="B15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1046,8 +1109,8 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="16"/>
       <c r="C16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1062,8 +1125,8 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="16"/>
-      <c r="B17" s="16"/>
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
       <c r="C17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1512,7 +1575,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
@@ -1529,7 +1592,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
+      <c r="A3" s="18"/>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
@@ -1544,7 +1607,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
+      <c r="A4" s="18"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
@@ -1559,7 +1622,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
+      <c r="A5" s="18"/>
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
@@ -1574,7 +1637,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1591,7 +1654,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
+      <c r="A7" s="18"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
@@ -1606,7 +1669,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
+      <c r="A8" s="18"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
@@ -1621,7 +1684,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
+      <c r="A9" s="18"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
@@ -1636,7 +1699,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8" t="s">
@@ -1653,7 +1716,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
@@ -1668,7 +1731,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
+      <c r="A12" s="18"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
@@ -1683,7 +1746,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
+      <c r="A13" s="18"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
@@ -1698,7 +1761,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
@@ -1715,7 +1778,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
+      <c r="A15" s="18"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
@@ -1730,7 +1793,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
@@ -1745,7 +1808,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
+      <c r="A17" s="18"/>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
@@ -1774,8 +1837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{382CD632-0A6C-274D-974D-E990EBE38F8D}">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1804,7 +1867,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1824,8 +1887,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="17"/>
-      <c r="B3" s="17" t="s">
+      <c r="A3" s="18"/>
+      <c r="B3" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1842,8 +1905,8 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="17"/>
-      <c r="B4" s="17"/>
+      <c r="A4" s="18"/>
+      <c r="B4" s="18"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1858,8 +1921,8 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="17"/>
+      <c r="A5" s="18"/>
+      <c r="B5" s="18"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
@@ -1874,7 +1937,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
+      <c r="A6" s="18"/>
       <c r="B6" s="4" t="s">
         <v>62</v>
       </c>
@@ -1892,7 +1955,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1912,8 +1975,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1930,8 +1993,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
+      <c r="A9" s="18"/>
+      <c r="B9" s="18"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1946,8 +2009,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
+      <c r="A10" s="18"/>
+      <c r="B10" s="18"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1962,7 +2025,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
+      <c r="A11" s="18"/>
       <c r="B11" s="4" t="s">
         <v>62</v>
       </c>
@@ -1980,7 +2043,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="18" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
@@ -2000,8 +2063,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17" t="s">
+      <c r="A13" s="18"/>
+      <c r="B13" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -2018,8 +2081,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
+      <c r="A14" s="18"/>
+      <c r="B14" s="18"/>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
@@ -2034,8 +2097,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
+      <c r="A15" s="18"/>
+      <c r="B15" s="18"/>
       <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
@@ -2050,7 +2113,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
+      <c r="A16" s="18"/>
       <c r="B16" s="4" t="s">
         <v>62</v>
       </c>
@@ -2068,7 +2131,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="17" t="s">
+      <c r="A17" s="18" t="s">
         <v>14</v>
       </c>
       <c r="B17" s="4" t="s">
@@ -2088,8 +2151,8 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
-      <c r="B18" s="17" t="s">
+      <c r="A18" s="18"/>
+      <c r="B18" s="18" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -2106,8 +2169,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="17"/>
+      <c r="A19" s="18"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="4" t="s">
         <v>10</v>
       </c>
@@ -2122,8 +2185,8 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="17"/>
+      <c r="A20" s="18"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
@@ -2138,7 +2201,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
+      <c r="A21" s="18"/>
       <c r="B21" s="4" t="s">
         <v>62</v>
       </c>
@@ -2172,10 +2235,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{359A555D-11EF-2C4B-8DAD-F0A6302620A2}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="A8" sqref="A8:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2241,7 +2304,7 @@
       <c r="B2" s="11">
         <v>0.87530068728522303</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="14">
         <v>0.57982780097661202</v>
       </c>
       <c r="D2" s="11">
@@ -2253,7 +2316,7 @@
       <c r="G2" s="5">
         <v>0.88780373612996799</v>
       </c>
-      <c r="H2" s="18">
+      <c r="H2" s="14">
         <v>0.52652391224719597</v>
       </c>
       <c r="I2" s="5">
@@ -2265,7 +2328,7 @@
       <c r="L2" s="5">
         <v>0.70258855468227299</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="14">
         <v>0.64359314820987201</v>
       </c>
       <c r="N2" s="5">
@@ -2277,7 +2340,7 @@
       <c r="Q2" s="5">
         <v>0.72721848190763505</v>
       </c>
-      <c r="R2" s="18">
+      <c r="R2" s="14">
         <v>0.220187328008842</v>
       </c>
       <c r="S2" s="5">
@@ -2435,22 +2498,37 @@
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
       <c r="B8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
         <v>67</v>
       </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>68</v>
       </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" t="s">
         <v>69</v>
+      </c>
+      <c r="J8" t="s">
+        <v>67</v>
+      </c>
+      <c r="K8" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>71</v>
       </c>
       <c r="B9" s="13">
         <v>0.58014632667510002</v>
@@ -2464,47 +2542,163 @@
       <c r="E9" s="13">
         <v>0.226835014050909</v>
       </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" s="13">
+        <v>0.58175855132687204</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0.52588994937270295</v>
+      </c>
+      <c r="J9" s="13">
+        <v>0.65545219329892701</v>
+      </c>
+      <c r="K9" s="5">
+        <v>0.21204022389264701</v>
+      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10">
+        <v>74</v>
+      </c>
+      <c r="B10" s="13">
+        <v>0.58175855132687204</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0.52588994937270295</v>
+      </c>
+      <c r="D10" s="13">
+        <v>0.65545219329892701</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.21204022389264701</v>
+      </c>
+      <c r="H10" s="19"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="20"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" s="14">
+        <v>0.57982780097661202</v>
+      </c>
+      <c r="C11" s="14">
+        <v>0.52652391224719597</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.64359314820987201</v>
+      </c>
+      <c r="E11" s="14">
+        <v>0.220187328008842</v>
+      </c>
+      <c r="H11" s="19"/>
+      <c r="I11" s="20"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="20"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>73</v>
+      </c>
+      <c r="B12" s="12">
+        <v>0.55767708199999999</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0.48329682886570802</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0.62732476061105102</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0.20549892835355499</v>
+      </c>
+      <c r="H12" s="19"/>
+      <c r="I12" s="20"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="20"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>75</v>
+      </c>
+      <c r="B13">
         <f>((B9-C2)/C2)*100</f>
         <v>5.4934533658356217E-2</v>
       </c>
-      <c r="C10">
+      <c r="C13">
         <f>((C9-H2)/H2)*100</f>
         <v>-1.4615380647808283</v>
       </c>
-      <c r="D10">
+      <c r="D13">
         <f>((D9-M2)/M2)*100</f>
         <v>0.47430152107765611</v>
       </c>
-      <c r="E10">
+      <c r="E13">
         <f>((E9-R2)/R2)*100</f>
         <v>3.0191047333114707</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>66</v>
-      </c>
-      <c r="B11">
+      <c r="G13" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13">
+        <f>((H9-C2)/C2)*100</f>
+        <v>0.33298685351203144</v>
+      </c>
+      <c r="I13">
+        <f>((I9-H2)/H2)*100</f>
+        <v>-0.12040533387881239</v>
+      </c>
+      <c r="J13">
+        <f>((J9-M2)/M2)*100</f>
+        <v>1.842630724401036</v>
+      </c>
+      <c r="K13">
+        <f>((K9-R2)/R2)*100</f>
+        <v>-3.7000785603192505</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14">
         <f>((B9-C4)/C4)*100</f>
         <v>4.0290780095388659</v>
       </c>
-      <c r="C11">
+      <c r="C14">
         <f>((C9-H4)/H4)*100</f>
         <v>7.3519489186830684</v>
       </c>
-      <c r="D11">
+      <c r="D14">
         <f>((D9-M5)/M5)*100</f>
         <v>3.0798975113802682</v>
       </c>
-      <c r="E11">
+      <c r="E14">
         <f>((E9-R3)/R3)*100</f>
         <v>10.382577597020793</v>
+      </c>
+      <c r="G14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14">
+        <f>((H9-C4)/C4)*100</f>
+        <v>4.3181744604796313</v>
+      </c>
+      <c r="I14">
+        <f>((I9-H4)/H4)*100</f>
+        <v>8.8130353776498964</v>
+      </c>
+      <c r="J14">
+        <f>((J9-M5)/M5)*100</f>
+        <v>4.4837115404911199</v>
+      </c>
+      <c r="K14">
+        <f>((K9-R3)/R3)*100</f>
+        <v>3.183128783931132</v>
       </c>
     </row>
   </sheetData>
@@ -2515,4 +2709,232 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6807B116-338D-DC43-B341-D2906F6EB460}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>81</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.58014632667510002</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.51882856484952999</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.64664572030138301</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.226835014050909</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.58175855132687204</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.52588994937270295</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.65545219329892701</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.21204022389264701</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.57982780097661202</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.52652391224719597</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.64359314820987201</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.220187328008842</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="5">
+        <v>0.55767708199999999</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0.48329682886570802</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0.62732476061105102</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.20549892835355499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="23"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
+      <c r="E6" s="23"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" s="21">
+        <f>((B2-B4)/B4)</f>
+        <v>5.4934533658356215E-4</v>
+      </c>
+      <c r="C7" s="21">
+        <f t="shared" ref="C7:E7" si="0">((C2-C4)/C4)</f>
+        <v>-1.4615380647808283E-2</v>
+      </c>
+      <c r="D7" s="21">
+        <f t="shared" si="0"/>
+        <v>4.7430152107765609E-3</v>
+      </c>
+      <c r="E7" s="21">
+        <f t="shared" si="0"/>
+        <v>3.0191047333114708E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="21">
+        <f>((B2-B5)/B5)</f>
+        <v>4.0290780095388661E-2</v>
+      </c>
+      <c r="C8" s="21">
+        <f t="shared" ref="C8:E8" si="1">((C2-C5)/C5)</f>
+        <v>7.3519489186830683E-2</v>
+      </c>
+      <c r="D8" s="21">
+        <f t="shared" si="1"/>
+        <v>3.0798975113802682E-2</v>
+      </c>
+      <c r="E8" s="21">
+        <f t="shared" si="1"/>
+        <v>0.10382577597020794</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B9" s="21">
+        <f>((B3-B4)/B4)</f>
+        <v>3.3298685351203145E-3</v>
+      </c>
+      <c r="C9" s="21">
+        <f t="shared" ref="C9:E9" si="2">((C3-C4)/C4)</f>
+        <v>-1.2040533387881239E-3</v>
+      </c>
+      <c r="D9" s="21">
+        <f t="shared" si="2"/>
+        <v>1.842630724401036E-2</v>
+      </c>
+      <c r="E9" s="21">
+        <f t="shared" si="2"/>
+        <v>-3.7000785603192504E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="21">
+        <f>((B3-B5)/B5)</f>
+        <v>4.3181744604796311E-2</v>
+      </c>
+      <c r="C10" s="21">
+        <f t="shared" ref="C10:E10" si="3">((C3-C5)/C5)</f>
+        <v>8.8130353776498971E-2</v>
+      </c>
+      <c r="D10" s="21">
+        <f t="shared" si="3"/>
+        <v>4.4837115404911199E-2</v>
+      </c>
+      <c r="E10" s="21">
+        <f t="shared" si="3"/>
+        <v>3.1831287839311322E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="24"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" s="21">
+        <f>((B3-B2)/B2)</f>
+        <v>2.7789965697307892E-3</v>
+      </c>
+      <c r="C12" s="21">
+        <f>((C3-C2)/C2)</f>
+        <v>1.361024623850633E-2</v>
+      </c>
+      <c r="D12" s="21">
+        <f t="shared" ref="C12:E12" si="4">((D3-D2)/D2)</f>
+        <v>1.3618698339856881E-2</v>
+      </c>
+      <c r="E12" s="21">
+        <f t="shared" si="4"/>
+        <v>-6.5222691567985033E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A11:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
chore: renamed env file
</commit_message>
<xml_diff>
--- a/report/model_comparison.xlsx
+++ b/report/model_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/gopikrishnan_srinivasan_ey_com/Documents/Gopi/UIUC/DLH/ConvolutionMedicalNer/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="267" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D5CD3D2-D553-CA40-A10C-7668DB38C65B}"/>
+  <xr:revisionPtr revIDLastSave="347" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E28D60B2-8A2D-E744-B5C8-37514AE9F573}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="-2940" windowWidth="51200" windowHeight="28800" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
+    <workbookView xWindow="30720" yWindow="-2940" windowWidth="51200" windowHeight="28800" activeTab="10" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
   </bookViews>
   <sheets>
     <sheet name="proposed" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,10 @@
     <sheet name="Baseline sorting" sheetId="6" r:id="rId5"/>
     <sheet name="Comparison - AUPRC" sheetId="7" r:id="rId6"/>
     <sheet name="Comparison - AUROC" sheetId="8" r:id="rId7"/>
+    <sheet name="Comparison - vs multi" sheetId="10" r:id="rId8"/>
+    <sheet name="Comparison - vs timeseries" sheetId="11" r:id="rId9"/>
+    <sheet name="Comparison - vs ablation" sheetId="12" r:id="rId10"/>
+    <sheet name="Comparison - AUPRC (2)" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Baseline sorting'!$P$1:$S$5</definedName>
@@ -45,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="39">
   <si>
     <t>Task</t>
   </si>
@@ -147,12 +151,30 @@
   </si>
   <si>
     <t>LOS &gt; 7</t>
+  </si>
+  <si>
+    <t>Proposed vs Multimodal</t>
+  </si>
+  <si>
+    <t>Proposed vs Timeseries</t>
+  </si>
+  <si>
+    <t>Glove vs Multimodal</t>
+  </si>
+  <si>
+    <t>Glove vs Timeseries</t>
+  </si>
+  <si>
+    <t>Glove vs Proposed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -267,7 +289,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -291,7 +313,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
@@ -316,6 +337,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -634,23 +658,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6912B902-6D37-5449-8B39-71DCD8060D35}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D14" activeCellId="3" sqref="D2 D6 D10 D14"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="3" width="19.1640625" style="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -664,274 +691,274 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13"/>
-      <c r="D2" s="5">
+      <c r="C2" s="12"/>
+      <c r="D2" s="23">
         <v>0.87530068728522303</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="23">
         <v>0.57982780097661202</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="23">
         <v>0.47647058823529398</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="23">
         <v>0.87565754692043296</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="23">
         <v>0.57975787210374596</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="24">
         <v>0.49450549450549403</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="13" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="23">
         <v>0.87006399242223997</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="23">
         <v>0.56660454860312803</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="23">
         <v>0.46262341325811002</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="13" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="24">
         <v>0.87878943078685301</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="24">
         <v>0.58014632667510002</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="23">
         <v>0.45468053491827598</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="5">
+      <c r="C6" s="12"/>
+      <c r="D6" s="23">
         <v>0.88780373612996799</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="23">
         <v>0.52652391224719597</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="23">
         <v>0.45614035087719301</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15" t="s">
+      <c r="A7" s="14"/>
+      <c r="B7" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="23">
         <v>0.88277697145621603</v>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="23">
         <v>0.50911558116714895</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="23">
         <v>0.43207126948774999</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="13" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="23">
         <v>0.88232595158949301</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="23">
         <v>0.51303461777177095</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="23">
         <v>0.44776119402984998</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="13" t="s">
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="23">
         <v>0.88463801363983896</v>
       </c>
-      <c r="E9" s="5">
-        <v>0.51882856484952999</v>
-      </c>
-      <c r="F9" s="12">
+      <c r="E9" s="23">
+        <v>0.51983490851077796</v>
+      </c>
+      <c r="F9" s="24">
         <v>0.45726495726495697</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="5">
+      <c r="C10" s="12"/>
+      <c r="D10" s="23">
         <v>0.70258855468227299</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="23">
         <v>0.64359314820987201</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="23">
         <v>0.57725947521865895</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15" t="s">
+      <c r="A11" s="14"/>
+      <c r="B11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="24">
         <v>0.702856581769842</v>
       </c>
-      <c r="E11" s="12">
+      <c r="E11" s="24">
         <v>0.64664572030138301</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="23">
         <v>0.55602923264311799</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="13" t="s">
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="23">
         <v>0.699181352047752</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="23">
         <v>0.644396926087205</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="23">
         <v>0.56094674556212998</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="13" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="5">
+      <c r="D13" s="23">
         <v>0.69989587514512697</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="23">
         <v>0.64207712275883899</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="23">
         <v>0.55840627829761502</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="5">
+      <c r="C14" s="12"/>
+      <c r="D14" s="23">
         <v>0.72721848190763505</v>
       </c>
-      <c r="E14" s="5">
-        <v>0.22731304632757199</v>
-      </c>
-      <c r="F14" s="5">
+      <c r="E14" s="23">
+        <v>0.21562758981911501</v>
+      </c>
+      <c r="F14" s="23">
         <v>5.3619302949061601E-2</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15" t="s">
+      <c r="A15" s="14"/>
+      <c r="B15" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="24">
         <v>0.73612815518677799</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="23">
         <v>0.22473590986289799</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="23">
         <v>1.11731843575419E-2</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
-      <c r="C16" s="13" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
+      <c r="C16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D16" s="23">
         <v>0.72345991139582499</v>
       </c>
-      <c r="E16" s="5">
-        <v>0.21963658925340199</v>
-      </c>
-      <c r="F16" s="5">
+      <c r="E16" s="24">
+        <v>0.23121145079482799</v>
+      </c>
+      <c r="F16" s="23">
         <v>1.6666666666666601E-2</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
-      <c r="C17" s="13" t="s">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
+      <c r="C17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="23">
         <v>0.72857653509265696</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="23">
         <v>0.226835014050909</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="24">
         <v>3.2786885245901599E-2</v>
       </c>
     </row>
@@ -947,7 +974,284 @@
     <mergeCell ref="B11:B13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0B1792-B3AF-E946-8847-4D8E02A72C8A}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="23">
+        <v>0.58014632667510002</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0.51983490851077796</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.64664572030138301</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.23121145079482799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.58175855132687204</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.52588994937270295</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.65545219329892701</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.21204022389264701</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="17">
+        <f>((B3-B2)/B2)</f>
+        <v>2.7789965697307892E-3</v>
+      </c>
+      <c r="C5" s="17">
+        <f>((C3-C2)/C2)</f>
+        <v>1.1648007401564194E-2</v>
+      </c>
+      <c r="D5" s="17">
+        <f t="shared" ref="D5:F5" si="0">((D3-D2)/D2)</f>
+        <v>1.3618698339856881E-2</v>
+      </c>
+      <c r="E5" s="17">
+        <f t="shared" si="0"/>
+        <v>-8.291642492738438E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6858C820-799C-8241-8B99-DAD6B7B6DDC1}">
+  <dimension ref="A1:E9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="23">
+        <v>0.58175855132687204</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0.52588994937270295</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.65545219329892701</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.21204022389264701</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.58014632667510002</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.51983490851077796</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.64664572030138301</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.23121145079482799</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="23">
+        <v>0.57982780097661202</v>
+      </c>
+      <c r="C4" s="23">
+        <v>0.52652391224719597</v>
+      </c>
+      <c r="D4" s="23">
+        <v>0.64359314820987201</v>
+      </c>
+      <c r="E4" s="23">
+        <v>0.21562758981911501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="17">
+        <f>((B3-B4)/B4)</f>
+        <v>5.4934533658356215E-4</v>
+      </c>
+      <c r="C6" s="17">
+        <f>((C3-C4)/C4)</f>
+        <v>-1.2704083481924769E-2</v>
+      </c>
+      <c r="D6" s="17">
+        <f>((D3-D4)/D4)</f>
+        <v>4.7430152107765609E-3</v>
+      </c>
+      <c r="E6" s="17">
+        <f>((E3-E4)/E4)</f>
+        <v>7.2272110395455086E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="17">
+        <f>((B2-B4)/B4)</f>
+        <v>3.3298685351203145E-3</v>
+      </c>
+      <c r="C7" s="17">
+        <f>((C2-C4)/C4)</f>
+        <v>-1.2040533387881239E-3</v>
+      </c>
+      <c r="D7" s="17">
+        <f>((D2-D4)/D4)</f>
+        <v>1.842630724401036E-2</v>
+      </c>
+      <c r="E7" s="17">
+        <f>((E2-E4)/E4)</f>
+        <v>-1.6636859547877678E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="17">
+        <f>((B2-B3)/B3)</f>
+        <v>2.7789965697307892E-3</v>
+      </c>
+      <c r="C9" s="17">
+        <f>((C2-C3)/C3)</f>
+        <v>1.1648007401564194E-2</v>
+      </c>
+      <c r="D9" s="17">
+        <f>((D2-D3)/D3)</f>
+        <v>1.3618698339856881E-2</v>
+      </c>
+      <c r="E9" s="17">
+        <f>((E2-E3)/E3)</f>
+        <v>-8.291642492738438E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A5:E5"/>
+    <mergeCell ref="A8:E8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1141,14 +1445,14 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -1169,250 +1473,250 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="9">
+      <c r="C2" s="25">
         <v>0.873989448</v>
       </c>
-      <c r="D2" s="9">
+      <c r="D2" s="25">
         <v>0.55767708199999999</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="25">
         <v>0.42813455700000003</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
+      <c r="A3" s="14"/>
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="12">
+      <c r="C3" s="24">
         <v>0.87530068728522303</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="24">
         <v>0.57982780097661202</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="23">
         <v>0.47246376811594198</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
+      <c r="A4" s="14"/>
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="23">
         <v>0.87519770464358104</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="23">
         <v>0.57818662871512605</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="24">
         <v>0.47647058823529398</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
+      <c r="A5" s="14"/>
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="23">
         <v>0.87328343906952099</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="23">
         <v>0.57552515759771194</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="23">
         <v>0.45588235294117602</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="14" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="23">
         <v>0.87717979930396195</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="23">
         <v>0.48329682886570802</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="23">
         <v>0.36613272311212802</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="15"/>
+      <c r="A7" s="14"/>
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7" s="24">
         <v>0.88780373612996799</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="24">
         <v>0.52652391224719597</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="24">
         <v>0.45614035087719301</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
+      <c r="A8" s="14"/>
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="23">
         <v>0.88387799054262794</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="23">
         <v>0.52074057278872599</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="23">
         <v>0.39069767441860398</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="23">
         <v>0.87679900744416805</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="23">
         <v>0.51472184249654396</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="23">
         <v>0.42857142857142799</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+      <c r="A10" s="14" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="23">
         <v>0.68930804987634497</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D10" s="23">
         <v>0.62732476061105102</v>
       </c>
-      <c r="E10" s="5">
+      <c r="E10" s="23">
         <v>0.53585842905929804</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="23">
         <v>0.70132707936795602</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="23">
         <v>0.64093450905905003</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="23">
         <v>0.54858934169278994</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
+      <c r="A12" s="14"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="23">
         <v>0.69839550612232504</v>
       </c>
-      <c r="D12" s="5">
+      <c r="D12" s="23">
         <v>0.63968225767197195</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="23">
         <v>0.53437500000000004</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="24">
         <v>0.70258855468227299</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="24">
         <v>0.64359314820987201</v>
       </c>
-      <c r="E13" s="12">
+      <c r="E13" s="24">
         <v>0.57725947521865895</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="23">
         <v>0.724200507757087</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="23">
         <v>0.20549892835355499</v>
       </c>
-      <c r="E14" s="5">
+      <c r="E14" s="23">
         <v>2.17983651226158E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
+      <c r="A15" s="14"/>
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="12">
+      <c r="C15" s="24">
         <v>0.72721848190763505</v>
       </c>
-      <c r="D15" s="5">
+      <c r="D15" s="23">
         <v>0.220187328008842</v>
       </c>
-      <c r="E15" s="5">
+      <c r="E15" s="23">
         <v>1.6483516483516401E-2</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="23">
         <v>0.72325409245457195</v>
       </c>
-      <c r="D16" s="12">
-        <v>0.22731304632757199</v>
-      </c>
-      <c r="E16" s="12">
+      <c r="D16" s="24">
+        <v>0.21562758981911501</v>
+      </c>
+      <c r="E16" s="24">
         <v>5.3619302949061601E-2</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="23">
         <v>0.71372661052441899</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="23">
         <v>0.20490147180395701</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="23">
         <v>1.6348773841961799E-2</v>
       </c>
     </row>
@@ -1424,7 +1728,7 @@
     <mergeCell ref="A10:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1462,13 +1766,13 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="5">
         <v>0.87530068728522303</v>
       </c>
@@ -1480,8 +1784,8 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="15"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="14"/>
+      <c r="B3" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1493,13 +1797,13 @@
       <c r="E3" s="5">
         <v>0.57975787210374596</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>0.49450549450549403</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="15"/>
-      <c r="B4" s="15"/>
+      <c r="A4" s="14"/>
+      <c r="B4" s="14"/>
       <c r="C4" s="4" t="s">
         <v>10</v>
       </c>
@@ -1514,12 +1818,12 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
+      <c r="A5" s="14"/>
+      <c r="B5" s="14"/>
       <c r="C5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>0.87878943078685301</v>
       </c>
       <c r="E5" s="5">
@@ -1530,7 +1834,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="15"/>
+      <c r="A6" s="14"/>
       <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1540,7 +1844,7 @@
       <c r="D6">
         <v>0.87769076915976596</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>0.58175855132687204</v>
       </c>
       <c r="F6" s="5">
@@ -1548,13 +1852,13 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="13"/>
+      <c r="C7" s="12"/>
       <c r="D7" s="5">
         <v>0.88780373612996799</v>
       </c>
@@ -1566,8 +1870,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1584,8 +1888,8 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
       <c r="C9" s="4" t="s">
         <v>10</v>
       </c>
@@ -1600,8 +1904,8 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
       <c r="C10" s="4" t="s">
         <v>11</v>
       </c>
@@ -1616,7 +1920,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="4" t="s">
         <v>18</v>
       </c>
@@ -1629,18 +1933,18 @@
       <c r="E11" s="5">
         <v>0.52588994937270295</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="11">
         <v>0.46220302375809902</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="5">
         <v>0.70258855468227299</v>
       </c>
@@ -1652,8 +1956,8 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1670,8 +1974,8 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="A14" s="14"/>
+      <c r="B14" s="14"/>
       <c r="C14" s="4" t="s">
         <v>10</v>
       </c>
@@ -1686,8 +1990,8 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="A15" s="14"/>
+      <c r="B15" s="14"/>
       <c r="C15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1702,31 +2006,31 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
+      <c r="A16" s="14"/>
       <c r="B16" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="11">
         <v>0.71348302180900203</v>
       </c>
-      <c r="E16" s="12">
+      <c r="E16" s="11">
         <v>0.65545219329892701</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>0.56099843993759702</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="13"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="5">
         <v>0.72721848190763505</v>
       </c>
@@ -1738,14 +2042,14 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15" t="s">
+      <c r="A18" s="14"/>
+      <c r="B18" s="14" t="s">
         <v>8</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="11">
         <v>0.73612815518677799</v>
       </c>
       <c r="E18" s="5">
@@ -1756,8 +2060,8 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="4" t="s">
         <v>10</v>
       </c>
@@ -1772,23 +2076,23 @@
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20" s="15"/>
-      <c r="B20" s="15"/>
+      <c r="A20" s="14"/>
+      <c r="B20" s="14"/>
       <c r="C20" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="5">
         <v>0.72857653509265696</v>
       </c>
-      <c r="E20" s="12">
+      <c r="E20" s="11">
         <v>0.226835014050909</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="11">
         <v>3.2786885245901599E-2</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
+      <c r="A21" s="14"/>
       <c r="B21" s="4" t="s">
         <v>18</v>
       </c>
@@ -1886,16 +2190,16 @@
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>0.87519770464358104</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="21">
         <v>0.57818662871512605</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>0.47647058823529398</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -1904,7 +2208,7 @@
       <c r="G2" s="5">
         <v>0.88780373612996799</v>
       </c>
-      <c r="H2" s="14">
+      <c r="H2" s="13">
         <v>0.52652391224719597</v>
       </c>
       <c r="I2" s="5">
@@ -1916,7 +2220,7 @@
       <c r="L2" s="5">
         <v>0.70258855468227299</v>
       </c>
-      <c r="M2" s="14">
+      <c r="M2" s="13">
         <v>0.64359314820987201</v>
       </c>
       <c r="N2" s="5">
@@ -1928,7 +2232,7 @@
       <c r="Q2" s="5">
         <v>0.72325409245457195</v>
       </c>
-      <c r="R2" s="22">
+      <c r="R2" s="21">
         <v>0.22731304632757199</v>
       </c>
       <c r="S2" s="5">
@@ -1936,13 +2240,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="5">
         <v>0.87530068728522303</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="22">
         <v>0.57982780097661202</v>
       </c>
       <c r="D3" s="5">
@@ -1998,7 +2302,7 @@
       <c r="D4" s="5">
         <v>0.45588235294117602</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="5">
@@ -2022,13 +2326,13 @@
       <c r="N4" s="5">
         <v>0.53585842905929804</v>
       </c>
-      <c r="P4" s="13" t="s">
+      <c r="P4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="Q4" s="5">
         <v>0.72721848190763505</v>
       </c>
-      <c r="R4" s="23">
+      <c r="R4" s="22">
         <v>0.220187328008842</v>
       </c>
       <c r="S4" s="5">
@@ -2039,13 +2343,13 @@
       <c r="A5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="11">
+      <c r="B5" s="10">
         <v>0.873989448</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="10">
         <v>0.55767708199999999</v>
       </c>
-      <c r="D5" s="11">
+      <c r="D5" s="10">
         <v>0.42813455700000003</v>
       </c>
       <c r="F5" s="8" t="s">
@@ -2060,7 +2364,7 @@
       <c r="I5" s="5">
         <v>0.36613272311212802</v>
       </c>
-      <c r="K5" s="13" t="s">
+      <c r="K5" s="12" t="s">
         <v>10</v>
       </c>
       <c r="L5" s="5">
@@ -2086,44 +2390,44 @@
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="H9" s="12"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="H9" s="11"/>
       <c r="I9" s="5"/>
-      <c r="J9" s="12"/>
+      <c r="J9" s="11"/>
       <c r="K9" s="5"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="5"/>
-      <c r="D10" s="12"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="5"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="17"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="16"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="14"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="16"/>
-      <c r="K11" s="17"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="16"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="16"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B12" s="11"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-      <c r="H12" s="16"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="16"/>
-      <c r="K12" s="17"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="16"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="16"/>
     </row>
   </sheetData>
   <autoFilter ref="P1:S5" xr:uid="{359A555D-11EF-2C4B-8DAD-F0A6302620A2}">
@@ -2141,28 +2445,30 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2170,33 +2476,33 @@
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="23">
         <v>0.58014632667510002</v>
       </c>
-      <c r="C2" s="5">
-        <v>0.51882856484952999</v>
-      </c>
-      <c r="D2" s="5">
+      <c r="C2" s="23">
+        <v>0.51983490851077796</v>
+      </c>
+      <c r="D2" s="23">
         <v>0.64664572030138301</v>
       </c>
-      <c r="E2" s="5">
-        <v>0.226835014050909</v>
+      <c r="E2" s="23">
+        <v>0.23121145079482799</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="23">
         <v>0.58175855132687204</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="23">
         <v>0.52588994937270295</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="23">
         <v>0.65545219329892701</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="23">
         <v>0.21204022389264701</v>
       </c>
     </row>
@@ -2204,155 +2510,385 @@
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="23">
         <v>0.57982780097661202</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="23">
         <v>0.52652391224719597</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="23">
         <v>0.64359314820987201</v>
       </c>
-      <c r="E4" s="5">
-        <v>0.22731304632757199</v>
+      <c r="E4" s="23">
+        <v>0.21562758981911501</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="23">
         <v>0.55767708199999999</v>
       </c>
+      <c r="C5" s="23">
+        <v>0.48329682886570802</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.62732476061105102</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0.20549892835355499</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="17">
+        <f>((B2-B4)/B4)</f>
+        <v>5.4934533658356215E-4</v>
+      </c>
+      <c r="C7" s="17">
+        <f t="shared" ref="C7:D7" si="0">((C2-C4)/C4)</f>
+        <v>-1.2704083481924769E-2</v>
+      </c>
+      <c r="D7" s="17">
+        <f t="shared" si="0"/>
+        <v>4.7430152107765609E-3</v>
+      </c>
+      <c r="E7" s="17">
+        <f>((E2-E4)/E4)</f>
+        <v>7.2272110395455086E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8" s="17">
+        <f>((B2-B5)/B5)</f>
+        <v>4.0290780095388661E-2</v>
+      </c>
+      <c r="C8" s="17">
+        <f t="shared" ref="C8:E8" si="1">((C2-C5)/C5)</f>
+        <v>7.5601736785288629E-2</v>
+      </c>
+      <c r="D8" s="17">
+        <f t="shared" si="1"/>
+        <v>3.0798975113802682E-2</v>
+      </c>
+      <c r="E8" s="17">
+        <f t="shared" si="1"/>
+        <v>0.12512241619593925</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="17">
+        <f>((B3-B4)/B4)</f>
+        <v>3.3298685351203145E-3</v>
+      </c>
+      <c r="C9" s="17">
+        <f t="shared" ref="C9:D9" si="2">((C3-C4)/C4)</f>
+        <v>-1.2040533387881239E-3</v>
+      </c>
+      <c r="D9" s="17">
+        <f t="shared" si="2"/>
+        <v>1.842630724401036E-2</v>
+      </c>
+      <c r="E9" s="17">
+        <f>((E3-E4)/E4)</f>
+        <v>-1.6636859547877678E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="17">
+        <f>((B3-B5)/B5)</f>
+        <v>4.3181744604796311E-2</v>
+      </c>
+      <c r="C10" s="17">
+        <f t="shared" ref="C10:E10" si="3">((C3-C5)/C5)</f>
+        <v>8.8130353776498971E-2</v>
+      </c>
+      <c r="D10" s="17">
+        <f t="shared" si="3"/>
+        <v>4.4837115404911199E-2</v>
+      </c>
+      <c r="E10" s="17">
+        <f t="shared" si="3"/>
+        <v>3.1831287839311322E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="17">
+        <f>((B3-B2)/B2)</f>
+        <v>2.7789965697307892E-3</v>
+      </c>
+      <c r="C12" s="17">
+        <f>((C3-C2)/C2)</f>
+        <v>1.1648007401564194E-2</v>
+      </c>
+      <c r="D12" s="17">
+        <f t="shared" ref="C12:E12" si="4">((D3-D2)/D2)</f>
+        <v>1.3618698339856881E-2</v>
+      </c>
+      <c r="E12" s="17">
+        <f t="shared" si="4"/>
+        <v>-8.291642492738438E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A6:E6"/>
+    <mergeCell ref="A11:E11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D43B48-8302-5940-A3EA-D2272996F125}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E12" sqref="A1:E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="5">
+        <v>0.87878943078685301</v>
+      </c>
+      <c r="C2" s="5">
+        <v>0.88463801399999997</v>
+      </c>
+      <c r="D2" s="5">
+        <v>0.702856581769842</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.73612815518677799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5">
+        <v>0.87769076915976596</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0.88211070260825897</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0.71348302180900203</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.72636501852534097</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.87530068728522303</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.88780373612996799</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0.70258855468227299</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.72721848190763505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0.873989448</v>
+      </c>
       <c r="C5" s="5">
-        <v>0.48329682886570802</v>
+        <v>0.87717979930396195</v>
       </c>
       <c r="D5" s="5">
-        <v>0.62732476061105102</v>
+        <v>0.68930804987634497</v>
       </c>
       <c r="E5" s="5">
-        <v>0.20549892835355499</v>
+        <v>0.724200507757087</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="18">
+      <c r="B7" s="17">
         <f>((B2-B4)/B4)</f>
-        <v>5.4934533658356215E-4</v>
-      </c>
-      <c r="C7" s="18">
-        <f t="shared" ref="C7:D7" si="0">((C2-C4)/C4)</f>
-        <v>-1.4615380647808283E-2</v>
-      </c>
-      <c r="D7" s="18">
+        <v>3.9857657514818607E-3</v>
+      </c>
+      <c r="C7" s="17">
+        <f t="shared" ref="C7:E7" si="0">((C2-C4)/C4)</f>
+        <v>-3.5657905020401713E-3</v>
+      </c>
+      <c r="D7" s="17">
         <f t="shared" si="0"/>
-        <v>4.7430152107765609E-3</v>
-      </c>
-      <c r="E7" s="18">
-        <f>((E2-E4)/E4)</f>
-        <v>-2.1029689425485667E-3</v>
+        <v>3.8148513206313152E-4</v>
+      </c>
+      <c r="E7" s="17">
+        <f t="shared" si="0"/>
+        <v>1.2251714582075992E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="18">
+      <c r="B8" s="17">
         <f>((B2-B5)/B5)</f>
-        <v>4.0290780095388661E-2</v>
-      </c>
-      <c r="C8" s="18">
+        <v>5.492037458618159E-3</v>
+      </c>
+      <c r="C8" s="17">
         <f t="shared" ref="C8:E8" si="1">((C2-C5)/C5)</f>
-        <v>7.3519489186830683E-2</v>
-      </c>
-      <c r="D8" s="18">
+        <v>8.5024925356877602E-3</v>
+      </c>
+      <c r="D8" s="17">
         <f t="shared" si="1"/>
-        <v>3.0798975113802682E-2</v>
-      </c>
-      <c r="E8" s="18">
+        <v>1.9655264284128848E-2</v>
+      </c>
+      <c r="E8" s="17">
         <f t="shared" si="1"/>
-        <v>0.10382577597020794</v>
+        <v>1.6470089846570213E-2</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="17">
         <f>((B3-B4)/B4)</f>
-        <v>3.3298685351203145E-3</v>
-      </c>
-      <c r="C9" s="18">
-        <f t="shared" ref="C9:D9" si="2">((C3-C4)/C4)</f>
-        <v>-1.2040533387881239E-3</v>
-      </c>
-      <c r="D9" s="18">
+        <v>2.7305837973872183E-3</v>
+      </c>
+      <c r="C9" s="17">
+        <f t="shared" ref="C9:E9" si="2">((C3-C4)/C4)</f>
+        <v>-6.4124910608346491E-3</v>
+      </c>
+      <c r="D9" s="17">
         <f t="shared" si="2"/>
-        <v>1.842630724401036E-2</v>
-      </c>
-      <c r="E9" s="18">
-        <f>((E3-E4)/E4)</f>
-        <v>-6.7188499215816697E-2</v>
+        <v>1.5506183603653733E-2</v>
+      </c>
+      <c r="E9" s="17">
+        <f t="shared" si="2"/>
+        <v>-1.1735996863766224E-3</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="18">
+      <c r="B10" s="17">
         <f>((B3-B5)/B5)</f>
-        <v>4.3181744604796311E-2</v>
-      </c>
-      <c r="C10" s="18">
+        <v>4.2349723652109336E-3</v>
+      </c>
+      <c r="C10" s="17">
         <f t="shared" ref="C10:E10" si="3">((C3-C5)/C5)</f>
-        <v>8.8130353776498971E-2</v>
-      </c>
-      <c r="D10" s="18">
+        <v>5.6213142484695467E-3</v>
+      </c>
+      <c r="D10" s="17">
         <f t="shared" si="3"/>
-        <v>4.4837115404911199E-2</v>
-      </c>
-      <c r="E10" s="18">
+        <v>3.5071361689441756E-2</v>
+      </c>
+      <c r="E10" s="17">
         <f t="shared" si="3"/>
-        <v>3.1831287839311322E-2</v>
+        <v>2.9888280180272865E-3</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
+      <c r="A11" s="20"/>
+      <c r="B11" s="20"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="18">
+      <c r="B12" s="17">
         <f>((B3-B2)/B2)</f>
-        <v>2.7789965697307892E-3</v>
-      </c>
-      <c r="C12" s="18">
+        <v>-1.2501989539215634E-3</v>
+      </c>
+      <c r="C12" s="17">
         <f>((C3-C2)/C2)</f>
-        <v>1.361024623850633E-2</v>
-      </c>
-      <c r="D12" s="18">
-        <f t="shared" ref="C12:E12" si="4">((D3-D2)/D2)</f>
-        <v>1.3618698339856881E-2</v>
-      </c>
-      <c r="E12" s="18">
+        <v>-2.856887621540764E-3</v>
+      </c>
+      <c r="D12" s="17">
+        <f t="shared" ref="D12:E12" si="4">((D3-D2)/D2)</f>
+        <v>1.5118930824268451E-2</v>
+      </c>
+      <c r="E12" s="17">
         <f t="shared" si="4"/>
-        <v>-6.5222691567985033E-2</v>
+        <v>-1.3262821959254932E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2365,34 +2901,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6D43B48-8302-5940-A3EA-D2272996F125}">
-  <dimension ref="A1:E12"/>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3F6BEA7-8A31-BF4D-81A5-77F1D1D2A323}">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G35" sqref="G35"/>
+      <selection activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="E1" s="18" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2400,197 +2937,176 @@
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5">
-        <v>0.87878943078685301</v>
-      </c>
-      <c r="C2" s="5">
-        <v>0.88463801399999997</v>
-      </c>
-      <c r="D2" s="5">
-        <v>0.702856581769842</v>
-      </c>
-      <c r="E2" s="5">
-        <v>0.73612815518677799</v>
+      <c r="B2" s="23">
+        <v>0.58014632667510002</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0.51983490851077796</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.64664572030138301</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.23121145079482799</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="5">
-        <v>0.87769076915976596</v>
-      </c>
-      <c r="C3" s="5">
-        <v>0.88211070260825897</v>
-      </c>
-      <c r="D3" s="5">
-        <v>0.71348302180900203</v>
-      </c>
-      <c r="E3" s="5">
-        <v>0.72636501852534097</v>
+        <v>21</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.57982780097661202</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.52652391224719597</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.64359314820987201</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.21562758981911501</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" s="5">
-        <v>0.87530068728522303</v>
-      </c>
-      <c r="C4" s="5">
-        <v>0.88780373612996799</v>
-      </c>
-      <c r="D4" s="5">
-        <v>0.70258855468227299</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.72721848190763505</v>
-      </c>
+      <c r="A4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="11">
-        <v>0.873989448</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0.87717979930396195</v>
-      </c>
-      <c r="D5" s="5">
-        <v>0.68930804987634497</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.724200507757087</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="18">
-        <f>((B2-B4)/B4)</f>
-        <v>3.9857657514818607E-3</v>
-      </c>
-      <c r="C7" s="18">
-        <f t="shared" ref="C7:E7" si="0">((C2-C4)/C4)</f>
-        <v>-3.5657905020401713E-3</v>
-      </c>
-      <c r="D7" s="18">
-        <f t="shared" si="0"/>
-        <v>3.8148513206313152E-4</v>
-      </c>
-      <c r="E7" s="18">
-        <f t="shared" si="0"/>
-        <v>1.2251714582075992E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="18">
-        <f>((B2-B5)/B5)</f>
-        <v>5.492037458618159E-3</v>
-      </c>
-      <c r="C8" s="18">
-        <f t="shared" ref="C8:E8" si="1">((C2-C5)/C5)</f>
-        <v>8.5024925356877602E-3</v>
-      </c>
-      <c r="D8" s="18">
-        <f t="shared" si="1"/>
-        <v>1.9655264284128848E-2</v>
-      </c>
-      <c r="E8" s="18">
-        <f t="shared" si="1"/>
-        <v>1.6470089846570213E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B9" s="18">
-        <f>((B3-B4)/B4)</f>
-        <v>2.7305837973872183E-3</v>
-      </c>
-      <c r="C9" s="18">
-        <f t="shared" ref="C9:E9" si="2">((C3-C4)/C4)</f>
-        <v>-6.4124910608346491E-3</v>
-      </c>
-      <c r="D9" s="18">
-        <f t="shared" si="2"/>
-        <v>1.5506183603653733E-2</v>
-      </c>
-      <c r="E9" s="18">
-        <f t="shared" si="2"/>
-        <v>-1.1735996863766224E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="18">
-        <f>((B3-B5)/B5)</f>
-        <v>4.2349723652109336E-3</v>
-      </c>
-      <c r="C10" s="18">
-        <f t="shared" ref="C10:E10" si="3">((C3-C5)/C5)</f>
-        <v>5.6213142484695467E-3</v>
-      </c>
-      <c r="D10" s="18">
-        <f t="shared" si="3"/>
-        <v>3.5071361689441756E-2</v>
-      </c>
-      <c r="E10" s="18">
-        <f t="shared" si="3"/>
-        <v>2.9888280180272865E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="21"/>
-      <c r="C11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="21"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="18">
-        <f>((B3-B2)/B2)</f>
-        <v>-1.2501989539215634E-3</v>
-      </c>
-      <c r="C12" s="18">
-        <f>((C3-C2)/C2)</f>
-        <v>-2.856887621540764E-3</v>
-      </c>
-      <c r="D12" s="18">
-        <f t="shared" ref="D12:E12" si="4">((D3-D2)/D2)</f>
-        <v>1.5118930824268451E-2</v>
-      </c>
-      <c r="E12" s="18">
-        <f t="shared" si="4"/>
-        <v>-1.3262821959254932E-2</v>
+        <v>34</v>
+      </c>
+      <c r="B5" s="17">
+        <f>((B2-B3)/B3)</f>
+        <v>5.4934533658356215E-4</v>
+      </c>
+      <c r="C5" s="17">
+        <f>((C2-C3)/C3)</f>
+        <v>-1.2704083481924769E-2</v>
+      </c>
+      <c r="D5" s="17">
+        <f>((D2-D3)/D3)</f>
+        <v>4.7430152107765609E-3</v>
+      </c>
+      <c r="E5" s="17">
+        <f>((E2-E3)/E3)</f>
+        <v>7.2272110395455086E-2</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A6:E6"/>
-    <mergeCell ref="A11:E11"/>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CF62D5A-CE5F-E349-9CFC-37168334DBF8}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="18" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="23">
+        <v>0.58014632667510002</v>
+      </c>
+      <c r="C2" s="23">
+        <v>0.51983490851077796</v>
+      </c>
+      <c r="D2" s="23">
+        <v>0.64664572030138301</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.23121145079482799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" s="23">
+        <v>0.55767708199999999</v>
+      </c>
+      <c r="C3" s="23">
+        <v>0.48329682886570802</v>
+      </c>
+      <c r="D3" s="23">
+        <v>0.62732476061105102</v>
+      </c>
+      <c r="E3" s="23">
+        <v>0.20549892835355499</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="17">
+        <f>((B2-B3)/B3)</f>
+        <v>4.0290780095388661E-2</v>
+      </c>
+      <c r="C5" s="17">
+        <f>((C2-C3)/C3)</f>
+        <v>7.5601736785288629E-2</v>
+      </c>
+      <c r="D5" s="17">
+        <f>((D2-D3)/D3)</f>
+        <v>3.0798975113802682E-2</v>
+      </c>
+      <c r="E5" s="17">
+        <f>((E2-E3)/E3)</f>
+        <v>0.12512241619593925</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A4:E4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: updated result slides
</commit_message>
<xml_diff>
--- a/report/model_comparison.xlsx
+++ b/report/model_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/gopikrishnan_srinivasan_ey_com/Documents/Gopi/UIUC/DLH/ConvolutionMedicalNer/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="347" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E28D60B2-8A2D-E744-B5C8-37514AE9F573}"/>
+  <xr:revisionPtr revIDLastSave="355" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB18A4F8-81AA-BD45-A9B9-F63475BB816B}"/>
   <bookViews>
-    <workbookView xWindow="30720" yWindow="-2940" windowWidth="51200" windowHeight="28800" activeTab="10" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
+    <workbookView xWindow="40" yWindow="760" windowWidth="28040" windowHeight="17440" firstSheet="4" activeTab="10" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
   </bookViews>
   <sheets>
     <sheet name="proposed" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Comparison - vs multi" sheetId="10" r:id="rId8"/>
     <sheet name="Comparison - vs timeseries" sheetId="11" r:id="rId9"/>
     <sheet name="Comparison - vs ablation" sheetId="12" r:id="rId10"/>
-    <sheet name="Comparison - AUPRC (2)" sheetId="13" r:id="rId11"/>
+    <sheet name="Comparison - Ablation" sheetId="13" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Baseline sorting'!$P$1:$S$5</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="41">
   <si>
     <t>Task</t>
   </si>
@@ -135,9 +135,6 @@
     <t>glove vs timeseries</t>
   </si>
   <si>
-    <t>Comparision %</t>
-  </si>
-  <si>
     <t>golve vs proposed</t>
   </si>
   <si>
@@ -166,6 +163,15 @@
   </si>
   <si>
     <t>Glove vs Proposed</t>
+  </si>
+  <si>
+    <t>Comparison %</t>
+  </si>
+  <si>
+    <t>Proposed vs Best Baseline</t>
+  </si>
+  <si>
+    <t>Glove vs Best Baseline</t>
   </si>
 </sst>
 </file>
@@ -983,7 +989,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -998,16 +1004,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1046,7 +1052,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -1055,7 +1061,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="17">
         <f>((B3-B2)/B2)</f>
@@ -1088,12 +1094,12 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="10.5" customWidth="1"/>
   </cols>
@@ -1103,16 +1109,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -1168,7 +1174,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="19"/>
@@ -1177,7 +1183,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="B6" s="17">
         <f>((B3-B4)/B4)</f>
@@ -1198,7 +1204,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B7" s="17">
         <f>((B2-B4)/B4)</f>
@@ -1226,7 +1232,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B9" s="17">
         <f>((B2-B3)/B3)</f>
@@ -2460,16 +2466,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2542,7 +2548,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -2551,7 +2557,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="17">
         <f>((B2-B4)/B4)</f>
@@ -2572,7 +2578,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B8" s="17">
         <f>((B2-B5)/B5)</f>
@@ -2593,7 +2599,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B9" s="17">
         <f>((B3-B4)/B4)</f>
@@ -2614,7 +2620,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B10" s="17">
         <f>((B3-B5)/B5)</f>
@@ -2642,7 +2648,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="17">
         <f>((B3-B2)/B2)</f>
@@ -2676,7 +2682,7 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E12" sqref="A1:E12"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2690,16 +2696,16 @@
         <v>3</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2772,7 +2778,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="19"/>
@@ -2872,7 +2878,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B12" s="17">
         <f>((B3-B2)/B2)</f>
@@ -2906,7 +2912,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+      <selection sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2921,16 +2927,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2969,7 +2975,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -2978,7 +2984,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5" s="17">
         <f>((B2-B3)/B3)</f>
@@ -3011,7 +3017,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3026,16 +3032,16 @@
         <v>4</v>
       </c>
       <c r="B1" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="E1" s="18" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" s="18" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -3074,7 +3080,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B4" s="19"/>
       <c r="C4" s="19"/>
@@ -3083,7 +3089,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5" s="17">
         <f>((B2-B3)/B3)</f>

</xml_diff>

<commit_message>
feat: updated presentation with results
</commit_message>
<xml_diff>
--- a/report/model_comparison.xlsx
+++ b/report/model_comparison.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://eyus-my.sharepoint.com/personal/gopikrishnan_srinivasan_ey_com/Documents/Gopi/UIUC/DLH/ConvolutionMedicalNer/report/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="355" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB18A4F8-81AA-BD45-A9B9-F63475BB816B}"/>
+  <xr:revisionPtr revIDLastSave="386" documentId="8_{A6862859-F872-8C4B-B32C-FD6475F8CA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{26077646-92EE-5942-8F37-ECC09C8E4A72}"/>
   <bookViews>
-    <workbookView xWindow="40" yWindow="760" windowWidth="28040" windowHeight="17440" firstSheet="4" activeTab="10" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
+    <workbookView xWindow="30720" yWindow="-2940" windowWidth="51200" windowHeight="28800" activeTab="10" xr2:uid="{CD2B21F4-F5A8-154B-B161-290B1A7A657F}"/>
   </bookViews>
   <sheets>
     <sheet name="proposed" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,8 @@
     <sheet name="Comparison - vs multi" sheetId="10" r:id="rId8"/>
     <sheet name="Comparison - vs timeseries" sheetId="11" r:id="rId9"/>
     <sheet name="Comparison - vs ablation" sheetId="12" r:id="rId10"/>
-    <sheet name="Comparison - Ablation" sheetId="13" r:id="rId11"/>
+    <sheet name="training hours" sheetId="14" r:id="rId11"/>
+    <sheet name="Comparison - Ablation" sheetId="13" r:id="rId12"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Baseline sorting'!$P$1:$S$5</definedName>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="51">
   <si>
     <t>Task</t>
   </si>
@@ -172,6 +173,36 @@
   </si>
   <si>
     <t>Glove vs Best Baseline</t>
+  </si>
+  <si>
+    <t>Average Training Time taken per epoch</t>
+  </si>
+  <si>
+    <t>Prediction Task</t>
+  </si>
+  <si>
+    <t>In-hospital Mortality</t>
+  </si>
+  <si>
+    <t>ICU Mortality</t>
+  </si>
+  <si>
+    <t>LOS &gt; 3 days</t>
+  </si>
+  <si>
+    <t>LOS &gt; 7 days</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16 seconds </t>
+  </si>
+  <si>
+    <t>11 seconds</t>
+  </si>
+  <si>
+    <t>12 seconds</t>
+  </si>
+  <si>
+    <t>15 seconds</t>
   </si>
 </sst>
 </file>
@@ -295,7 +326,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -332,6 +363,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -704,13 +738,13 @@
         <v>7</v>
       </c>
       <c r="C2" s="12"/>
-      <c r="D2" s="23">
+      <c r="D2" s="24">
         <v>0.87530068728522303</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>0.57982780097661202</v>
       </c>
-      <c r="F2" s="23">
+      <c r="F2" s="24">
         <v>0.47647058823529398</v>
       </c>
     </row>
@@ -722,13 +756,13 @@
       <c r="C3" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>0.87565754692043296</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>0.57975787210374596</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="25">
         <v>0.49450549450549403</v>
       </c>
     </row>
@@ -738,13 +772,13 @@
       <c r="C4" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="24">
         <v>0.87006399242223997</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="24">
         <v>0.56660454860312803</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="24">
         <v>0.46262341325811002</v>
       </c>
     </row>
@@ -754,13 +788,13 @@
       <c r="C5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="24">
+      <c r="D5" s="25">
         <v>0.87878943078685301</v>
       </c>
-      <c r="E5" s="24">
+      <c r="E5" s="25">
         <v>0.58014632667510002</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="24">
         <v>0.45468053491827598</v>
       </c>
     </row>
@@ -772,13 +806,13 @@
         <v>7</v>
       </c>
       <c r="C6" s="12"/>
-      <c r="D6" s="23">
+      <c r="D6" s="24">
         <v>0.88780373612996799</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="24">
         <v>0.52652391224719597</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="24">
         <v>0.45614035087719301</v>
       </c>
     </row>
@@ -790,13 +824,13 @@
       <c r="C7" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="23">
+      <c r="D7" s="24">
         <v>0.88277697145621603</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="24">
         <v>0.50911558116714895</v>
       </c>
-      <c r="F7" s="23">
+      <c r="F7" s="24">
         <v>0.43207126948774999</v>
       </c>
     </row>
@@ -806,13 +840,13 @@
       <c r="C8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="24">
         <v>0.88232595158949301</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="24">
         <v>0.51303461777177095</v>
       </c>
-      <c r="F8" s="23">
+      <c r="F8" s="24">
         <v>0.44776119402984998</v>
       </c>
     </row>
@@ -822,13 +856,13 @@
       <c r="C9" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="24">
         <v>0.88463801363983896</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="24">
         <v>0.51983490851077796</v>
       </c>
-      <c r="F9" s="24">
+      <c r="F9" s="25">
         <v>0.45726495726495697</v>
       </c>
     </row>
@@ -840,13 +874,13 @@
         <v>7</v>
       </c>
       <c r="C10" s="12"/>
-      <c r="D10" s="23">
+      <c r="D10" s="24">
         <v>0.70258855468227299</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="24">
         <v>0.64359314820987201</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="24">
         <v>0.57725947521865895</v>
       </c>
     </row>
@@ -858,13 +892,13 @@
       <c r="C11" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="25">
         <v>0.702856581769842</v>
       </c>
-      <c r="E11" s="24">
+      <c r="E11" s="25">
         <v>0.64664572030138301</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="24">
         <v>0.55602923264311799</v>
       </c>
     </row>
@@ -874,13 +908,13 @@
       <c r="C12" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="24">
         <v>0.699181352047752</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="24">
         <v>0.644396926087205</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="24">
         <v>0.56094674556212998</v>
       </c>
     </row>
@@ -890,13 +924,13 @@
       <c r="C13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="23">
+      <c r="D13" s="24">
         <v>0.69989587514512697</v>
       </c>
-      <c r="E13" s="23">
+      <c r="E13" s="24">
         <v>0.64207712275883899</v>
       </c>
-      <c r="F13" s="23">
+      <c r="F13" s="24">
         <v>0.55840627829761502</v>
       </c>
     </row>
@@ -908,13 +942,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="12"/>
-      <c r="D14" s="23">
+      <c r="D14" s="24">
         <v>0.72721848190763505</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="24">
         <v>0.21562758981911501</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="24">
         <v>5.3619302949061601E-2</v>
       </c>
     </row>
@@ -926,13 +960,13 @@
       <c r="C15" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="25">
         <v>0.73612815518677799</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="24">
         <v>0.22473590986289799</v>
       </c>
-      <c r="F15" s="23">
+      <c r="F15" s="24">
         <v>1.11731843575419E-2</v>
       </c>
     </row>
@@ -942,13 +976,13 @@
       <c r="C16" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="24">
         <v>0.72345991139582499</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="25">
         <v>0.23121145079482799</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="24">
         <v>1.6666666666666601E-2</v>
       </c>
     </row>
@@ -958,13 +992,13 @@
       <c r="C17" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="24">
         <v>0.72857653509265696</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="24">
         <v>0.226835014050909</v>
       </c>
-      <c r="F17" s="24">
+      <c r="F17" s="25">
         <v>3.2786885245901599E-2</v>
       </c>
     </row>
@@ -988,8 +1022,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0B1792-B3AF-E946-8847-4D8E02A72C8A}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1000,19 +1034,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1020,16 +1054,16 @@
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="24">
         <v>0.58014632667510002</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="24">
         <v>0.51983490851077796</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="24">
         <v>0.64664572030138301</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>0.23121145079482799</v>
       </c>
     </row>
@@ -1037,27 +1071,27 @@
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>0.58175855132687204</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
         <v>0.52588994937270295</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>0.65545219329892701</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>0.21204022389264701</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -1090,10 +1124,69 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE13A246-A8D2-A445-80A3-300A52F19EA4}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="2" max="2" width="33.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="18" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6858C820-799C-8241-8B99-DAD6B7B6DDC1}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="A8" sqref="A8:E8"/>
     </sheetView>
   </sheetViews>
@@ -1105,19 +1198,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1125,16 +1218,16 @@
       <c r="A2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="24">
         <v>0.58175855132687204</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="24">
         <v>0.52588994937270295</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="24">
         <v>0.65545219329892701</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>0.21204022389264701</v>
       </c>
     </row>
@@ -1142,16 +1235,16 @@
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>0.58014632667510002</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
         <v>0.51983490851077796</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>0.64664572030138301</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>0.23121145079482799</v>
       </c>
     </row>
@@ -1159,27 +1252,27 @@
       <c r="A4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="24">
         <v>0.57982780097661202</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="24">
         <v>0.52652391224719597</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="24">
         <v>0.64359314820987201</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="24">
         <v>0.21562758981911501</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="19"/>
-      <c r="C5" s="19"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
@@ -1224,11 +1317,11 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
@@ -1485,13 +1578,13 @@
       <c r="B2" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="26">
         <v>0.873989448</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="26">
         <v>0.55767708199999999</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="26">
         <v>0.42813455700000003</v>
       </c>
     </row>
@@ -1500,13 +1593,13 @@
       <c r="B3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="25">
         <v>0.87530068728522303</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="25">
         <v>0.57982780097661202</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>0.47246376811594198</v>
       </c>
     </row>
@@ -1515,13 +1608,13 @@
       <c r="B4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="24">
         <v>0.87519770464358104</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="24">
         <v>0.57818662871512605</v>
       </c>
-      <c r="E4" s="24">
+      <c r="E4" s="25">
         <v>0.47647058823529398</v>
       </c>
     </row>
@@ -1530,13 +1623,13 @@
       <c r="B5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="24">
         <v>0.87328343906952099</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="24">
         <v>0.57552515759771194</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="24">
         <v>0.45588235294117602</v>
       </c>
     </row>
@@ -1547,13 +1640,13 @@
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="23">
+      <c r="C6" s="24">
         <v>0.87717979930396195</v>
       </c>
-      <c r="D6" s="23">
+      <c r="D6" s="24">
         <v>0.48329682886570802</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="24">
         <v>0.36613272311212802</v>
       </c>
     </row>
@@ -1562,13 +1655,13 @@
       <c r="B7" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="24">
+      <c r="C7" s="25">
         <v>0.88780373612996799</v>
       </c>
-      <c r="D7" s="24">
+      <c r="D7" s="25">
         <v>0.52652391224719597</v>
       </c>
-      <c r="E7" s="24">
+      <c r="E7" s="25">
         <v>0.45614035087719301</v>
       </c>
     </row>
@@ -1577,13 +1670,13 @@
       <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="23">
+      <c r="C8" s="24">
         <v>0.88387799054262794</v>
       </c>
-      <c r="D8" s="23">
+      <c r="D8" s="24">
         <v>0.52074057278872599</v>
       </c>
-      <c r="E8" s="23">
+      <c r="E8" s="24">
         <v>0.39069767441860398</v>
       </c>
     </row>
@@ -1592,13 +1685,13 @@
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="23">
+      <c r="C9" s="24">
         <v>0.87679900744416805</v>
       </c>
-      <c r="D9" s="23">
+      <c r="D9" s="24">
         <v>0.51472184249654396</v>
       </c>
-      <c r="E9" s="23">
+      <c r="E9" s="24">
         <v>0.42857142857142799</v>
       </c>
     </row>
@@ -1609,13 +1702,13 @@
       <c r="B10" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="23">
+      <c r="C10" s="24">
         <v>0.68930804987634497</v>
       </c>
-      <c r="D10" s="23">
+      <c r="D10" s="24">
         <v>0.62732476061105102</v>
       </c>
-      <c r="E10" s="23">
+      <c r="E10" s="24">
         <v>0.53585842905929804</v>
       </c>
     </row>
@@ -1624,13 +1717,13 @@
       <c r="B11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="24">
         <v>0.70132707936795602</v>
       </c>
-      <c r="D11" s="23">
+      <c r="D11" s="24">
         <v>0.64093450905905003</v>
       </c>
-      <c r="E11" s="23">
+      <c r="E11" s="24">
         <v>0.54858934169278994</v>
       </c>
     </row>
@@ -1639,13 +1732,13 @@
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="23">
+      <c r="C12" s="24">
         <v>0.69839550612232504</v>
       </c>
-      <c r="D12" s="23">
+      <c r="D12" s="24">
         <v>0.63968225767197195</v>
       </c>
-      <c r="E12" s="23">
+      <c r="E12" s="24">
         <v>0.53437500000000004</v>
       </c>
     </row>
@@ -1654,13 +1747,13 @@
       <c r="B13" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="24">
+      <c r="C13" s="25">
         <v>0.70258855468227299</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="25">
         <v>0.64359314820987201</v>
       </c>
-      <c r="E13" s="24">
+      <c r="E13" s="25">
         <v>0.57725947521865895</v>
       </c>
     </row>
@@ -1671,13 +1764,13 @@
       <c r="B14" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="23">
+      <c r="C14" s="24">
         <v>0.724200507757087</v>
       </c>
-      <c r="D14" s="23">
+      <c r="D14" s="24">
         <v>0.20549892835355499</v>
       </c>
-      <c r="E14" s="23">
+      <c r="E14" s="24">
         <v>2.17983651226158E-2</v>
       </c>
     </row>
@@ -1686,13 +1779,13 @@
       <c r="B15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C15" s="25">
         <v>0.72721848190763505</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="24">
         <v>0.220187328008842</v>
       </c>
-      <c r="E15" s="23">
+      <c r="E15" s="24">
         <v>1.6483516483516401E-2</v>
       </c>
     </row>
@@ -1701,13 +1794,13 @@
       <c r="B16" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="24">
         <v>0.72325409245457195</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="25">
         <v>0.21562758981911501</v>
       </c>
-      <c r="E16" s="24">
+      <c r="E16" s="25">
         <v>5.3619302949061601E-2</v>
       </c>
     </row>
@@ -1716,13 +1809,13 @@
       <c r="B17" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="24">
         <v>0.71372661052441899</v>
       </c>
-      <c r="D17" s="23">
+      <c r="D17" s="24">
         <v>0.20490147180395701</v>
       </c>
-      <c r="E17" s="23">
+      <c r="E17" s="24">
         <v>1.6348773841961799E-2</v>
       </c>
     </row>
@@ -1743,7 +1836,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2202,7 +2295,7 @@
       <c r="B2" s="9">
         <v>0.87519770464358104</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="22">
         <v>0.57818662871512605</v>
       </c>
       <c r="D2" s="9">
@@ -2238,7 +2331,7 @@
       <c r="Q2" s="5">
         <v>0.72325409245457195</v>
       </c>
-      <c r="R2" s="21">
+      <c r="R2" s="22">
         <v>0.22731304632757199</v>
       </c>
       <c r="S2" s="5">
@@ -2252,7 +2345,7 @@
       <c r="B3" s="5">
         <v>0.87530068728522303</v>
       </c>
-      <c r="C3" s="22">
+      <c r="C3" s="23">
         <v>0.57982780097661202</v>
       </c>
       <c r="D3" s="5">
@@ -2338,7 +2431,7 @@
       <c r="Q4" s="5">
         <v>0.72721848190763505</v>
       </c>
-      <c r="R4" s="22">
+      <c r="R4" s="23">
         <v>0.220187328008842</v>
       </c>
       <c r="S4" s="5">
@@ -2462,19 +2555,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2482,16 +2575,16 @@
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="24">
         <v>0.58014632667510002</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="24">
         <v>0.51983490851077796</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="24">
         <v>0.64664572030138301</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>0.23121145079482799</v>
       </c>
     </row>
@@ -2499,16 +2592,16 @@
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>0.58175855132687204</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
         <v>0.52588994937270295</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>0.65545219329892701</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>0.21204022389264701</v>
       </c>
     </row>
@@ -2516,16 +2609,16 @@
       <c r="A4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="23">
+      <c r="B4" s="24">
         <v>0.57982780097661202</v>
       </c>
-      <c r="C4" s="23">
+      <c r="C4" s="24">
         <v>0.52652391224719597</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="24">
         <v>0.64359314820987201</v>
       </c>
-      <c r="E4" s="23">
+      <c r="E4" s="24">
         <v>0.21562758981911501</v>
       </c>
     </row>
@@ -2533,27 +2626,27 @@
       <c r="A5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="23">
+      <c r="B5" s="24">
         <v>0.55767708199999999</v>
       </c>
-      <c r="C5" s="23">
+      <c r="C5" s="24">
         <v>0.48329682886570802</v>
       </c>
-      <c r="D5" s="23">
+      <c r="D5" s="24">
         <v>0.62732476061105102</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="24">
         <v>0.20549892835355499</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -2640,11 +2733,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -2692,19 +2785,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2777,13 +2870,13 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
@@ -2870,11 +2963,11 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
@@ -2923,19 +3016,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2943,16 +3036,16 @@
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="24">
         <v>0.58014632667510002</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="24">
         <v>0.51983490851077796</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="24">
         <v>0.64664572030138301</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>0.23121145079482799</v>
       </c>
     </row>
@@ -2960,27 +3053,27 @@
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>0.57982780097661202</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
         <v>0.52652391224719597</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>0.64359314820987201</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>0.21562758981911501</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
@@ -3028,19 +3121,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="19" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="19" t="s">
         <v>32</v>
       </c>
     </row>
@@ -3048,16 +3141,16 @@
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="23">
+      <c r="B2" s="24">
         <v>0.58014632667510002</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="24">
         <v>0.51983490851077796</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="24">
         <v>0.64664572030138301</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>0.23121145079482799</v>
       </c>
     </row>
@@ -3065,27 +3158,27 @@
       <c r="A3" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="23">
+      <c r="B3" s="24">
         <v>0.55767708199999999</v>
       </c>
-      <c r="C3" s="23">
+      <c r="C3" s="24">
         <v>0.48329682886570802</v>
       </c>
-      <c r="D3" s="23">
+      <c r="D3" s="24">
         <v>0.62732476061105102</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="24">
         <v>0.20549892835355499</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B4" s="19"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">

</xml_diff>